<commit_message>
update llm results after fixing bug
</commit_message>
<xml_diff>
--- a/llm_warnings_per_program.xlsx
+++ b/llm_warnings_per_program.xlsx
@@ -562,58 +562,58 @@
         <v>7460</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>15</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J4" s="2" t="n">
         <v>9</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="Q4" s="2" t="n">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="R4" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S4" s="2" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="T4" s="2" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -626,19 +626,19 @@
         <v>8047</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>15</v>
@@ -647,37 +647,37 @@
         <v>39</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O5" s="2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P5" s="2" t="n">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="Q5" s="2" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R5" s="2" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S5" s="2" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="T5" s="2" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -690,58 +690,58 @@
         <v>5859</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>11</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>6</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M6" s="2" t="n">
         <v>249</v>
       </c>
       <c r="N6" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O6" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P6" s="2" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Q6" s="2" t="n">
         <v>35</v>
       </c>
       <c r="R6" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="T6" s="2" t="n">
         <v>6</v>
-      </c>
-      <c r="T6" s="2" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -754,58 +754,58 @@
         <v>13848</v>
       </c>
       <c r="C7" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>215</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>511</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="P7" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q7" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="R7" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="S7" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="D7" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>59</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>59</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>23</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>62</v>
-      </c>
-      <c r="J7" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="K7" s="2" t="n">
-        <v>219</v>
-      </c>
-      <c r="L7" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="M7" s="2" t="n">
-        <v>499</v>
-      </c>
-      <c r="N7" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="O7" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="P7" s="2" t="n">
-        <v>91</v>
-      </c>
-      <c r="Q7" s="2" t="n">
-        <v>113</v>
-      </c>
-      <c r="R7" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="S7" s="2" t="n">
-        <v>10</v>
-      </c>
       <c r="T7" s="2" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -818,13 +818,13 @@
         <v>14423</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>28</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>56</v>
@@ -836,34 +836,34 @@
         <v>24</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="L8" s="2" t="n">
         <v>5</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>574</v>
+        <v>580</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O8" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P8" s="2" t="n">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="Q8" s="2" t="n">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="R8" s="2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S8" s="2" t="n">
         <v>9</v>
@@ -885,55 +885,55 @@
         <v>5</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G9" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="J9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="H9" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="I9" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="J9" s="2" t="n">
-        <v>12</v>
-      </c>
       <c r="K9" s="2" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="N9" s="2" t="n">
         <v>3</v>
       </c>
       <c r="O9" s="2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P9" s="2" t="n">
         <v>46</v>
       </c>
       <c r="Q9" s="2" t="n">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R9" s="2" t="n">
         <v>2</v>
       </c>
       <c r="S9" s="2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T9" s="2" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -946,58 +946,58 @@
         <v>8299</v>
       </c>
       <c r="C10" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D10" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E10" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F10" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G10" t="n">
         <v>14</v>
       </c>
       <c r="H10" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I10" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J10" t="n">
         <v>9</v>
       </c>
       <c r="K10" t="n">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M10" t="n">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="N10" t="n">
         <v>2</v>
       </c>
       <c r="O10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P10" t="n">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="Q10" t="n">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="R10" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="S10" t="n">
         <v>7</v>
       </c>
       <c r="T10" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -1119,58 +1119,58 @@
         <v>7280</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>11</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="J16" s="2" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="N16" s="2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O16" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P16" s="2" t="n">
         <v>47</v>
       </c>
       <c r="Q16" s="2" t="n">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="R16" s="2" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S16" s="2" t="n">
         <v>7</v>
       </c>
       <c r="T16" s="2" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17">
@@ -1183,58 +1183,58 @@
         <v>7757</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H17" s="2" t="n">
         <v>20</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J17" s="2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="N17" s="2" t="n">
         <v>4</v>
       </c>
       <c r="O17" s="2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P17" s="2" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q17" s="2" t="n">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="R17" s="2" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="S17" s="2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T17" s="2" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
@@ -1250,25 +1250,25 @@
         <v>1</v>
       </c>
       <c r="D18" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="G18" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="E18" s="2" t="n">
-        <v>32</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>16</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <v>8</v>
-      </c>
       <c r="H18" s="2" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J18" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K18" s="2" t="n">
         <v>100</v>
@@ -1277,28 +1277,28 @@
         <v>2</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="N18" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O18" s="2" t="n">
         <v>3</v>
       </c>
       <c r="P18" s="2" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q18" s="2" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="R18" s="2" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="S18" s="2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T18" s="2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -1311,58 +1311,58 @@
         <v>12993</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H19" s="2" t="n">
         <v>39</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J19" s="2" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="K19" s="2" t="n">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="N19" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O19" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P19" s="2" t="n">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="Q19" s="2" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R19" s="2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="S19" s="2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T19" s="2" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20">
@@ -1375,58 +1375,58 @@
         <v>13484</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>52</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J20" s="2" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="K20" s="2" t="n">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="L20" s="2" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M20" s="2" t="n">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="N20" s="2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O20" s="2" t="n">
         <v>4</v>
       </c>
       <c r="P20" s="2" t="n">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="Q20" s="2" t="n">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="R20" s="2" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S20" s="2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="T20" s="2" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21">
@@ -1439,58 +1439,58 @@
         <v>6906</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I21" s="2" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J21" s="2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K21" s="2" t="n">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="L21" s="2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M21" s="2" t="n">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N21" s="2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O21" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="P21" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q21" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="R21" s="2" t="n">
         <v>7</v>
-      </c>
-      <c r="P21" s="2" t="n">
-        <v>40</v>
-      </c>
-      <c r="Q21" s="2" t="n">
-        <v>49</v>
-      </c>
-      <c r="R21" s="2" t="n">
-        <v>9</v>
       </c>
       <c r="S21" s="2" t="n">
         <v>8</v>
       </c>
       <c r="T21" s="2" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22">
@@ -1503,58 +1503,58 @@
         <v>8290</v>
       </c>
       <c r="C22" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D22" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E22" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F22" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G22" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H22" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I22" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J22" t="n">
+        <v>8</v>
+      </c>
+      <c r="K22" t="n">
+        <v>140</v>
+      </c>
+      <c r="L22" t="n">
+        <v>2</v>
+      </c>
+      <c r="M22" t="n">
+        <v>300</v>
+      </c>
+      <c r="N22" t="n">
+        <v>3</v>
+      </c>
+      <c r="O22" t="n">
+        <v>5</v>
+      </c>
+      <c r="P22" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>39</v>
+      </c>
+      <c r="R22" t="n">
         <v>13</v>
       </c>
-      <c r="K22" t="n">
-        <v>134</v>
-      </c>
-      <c r="L22" t="n">
-        <v>3</v>
-      </c>
-      <c r="M22" t="n">
-        <v>312</v>
-      </c>
-      <c r="N22" t="n">
-        <v>3</v>
-      </c>
-      <c r="O22" t="n">
-        <v>5</v>
-      </c>
-      <c r="P22" t="n">
-        <v>47</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>46</v>
-      </c>
-      <c r="R22" t="n">
-        <v>8</v>
-      </c>
       <c r="S22" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T22" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25">
@@ -1679,22 +1679,22 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J28" s="2" t="n">
         <v>0</v>
@@ -1709,7 +1709,7 @@
         <v>57</v>
       </c>
       <c r="N28" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O28" s="2" t="n">
         <v>2</v>
@@ -1718,10 +1718,10 @@
         <v>11</v>
       </c>
       <c r="Q28" s="2" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="R28" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S28" s="2" t="n">
         <v>2</v>
@@ -1746,31 +1746,31 @@
         <v>0</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I29" s="2" t="n">
         <v>11</v>
       </c>
       <c r="J29" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K29" s="2" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L29" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M29" s="2" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="N29" s="2" t="n">
         <v>0</v>
@@ -1779,16 +1779,16 @@
         <v>3</v>
       </c>
       <c r="P29" s="2" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="Q29" s="2" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="R29" s="2" t="n">
         <v>10</v>
       </c>
       <c r="S29" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T29" s="2" t="n">
         <v>1</v>
@@ -1810,16 +1810,16 @@
         <v>0</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I30" s="2" t="n">
         <v>6</v>
@@ -1828,28 +1828,28 @@
         <v>0</v>
       </c>
       <c r="K30" s="2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L30" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M30" s="2" t="n">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="N30" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O30" s="2" t="n">
         <v>1</v>
       </c>
       <c r="P30" s="2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q30" s="2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R30" s="2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="S30" s="2" t="n">
         <v>1</v>
@@ -1871,28 +1871,28 @@
         <v>0</v>
       </c>
       <c r="D31" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="E31" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="F31" s="2" t="n">
-        <v>47</v>
-      </c>
-      <c r="G31" s="2" t="n">
-        <v>27</v>
-      </c>
       <c r="H31" s="2" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I31" s="2" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J31" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K31" s="2" t="n">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="L31" s="2" t="n">
         <v>1</v>
@@ -1901,19 +1901,19 @@
         <v>107</v>
       </c>
       <c r="N31" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O31" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P31" s="2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q31" s="2" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R31" s="2" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="S31" s="2" t="n">
         <v>8</v>
@@ -1932,58 +1932,58 @@
         <v>6954</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="J32" s="2" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K32" s="2" t="n">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="L32" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32" s="2" t="n">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="N32" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O32" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P32" s="2" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q32" s="2" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R32" s="2" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="S32" s="2" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="T32" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1999,52 +1999,52 @@
         <v>0</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>12</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H33" s="2" t="n">
         <v>15</v>
       </c>
       <c r="I33" s="2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J33" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K33" s="2" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L33" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="2" t="n">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="N33" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O33" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P33" s="2" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="Q33" s="2" t="n">
         <v>15</v>
       </c>
       <c r="R33" s="2" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S33" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T33" s="2" t="n">
         <v>1</v>
@@ -2066,31 +2066,31 @@
         <v>1</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G34" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H34" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L34" t="n">
         <v>0</v>
       </c>
       <c r="M34" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="N34" t="n">
         <v>1</v>
@@ -2099,13 +2099,13 @@
         <v>1</v>
       </c>
       <c r="P34" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Q34" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="R34" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S34" t="n">
         <v>2</v>
@@ -2239,31 +2239,31 @@
         <v>0</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H40" s="2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I40" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J40" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K40" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M40" s="2" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N40" s="2" t="n">
         <v>1</v>
@@ -2275,10 +2275,10 @@
         <v>7</v>
       </c>
       <c r="Q40" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R40" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S40" s="2" t="n">
         <v>0</v>
@@ -2300,7 +2300,7 @@
         <v>0</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E41" s="2" t="n">
         <v>3</v>
@@ -2312,43 +2312,43 @@
         <v>5</v>
       </c>
       <c r="H41" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="I41" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J41" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K41" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="N41" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O41" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="P41" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q41" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="R41" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="I41" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="J41" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="K41" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="L41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O41" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="P41" s="2" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q41" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="R41" s="2" t="n">
-        <v>5</v>
-      </c>
       <c r="S41" s="2" t="n">
         <v>0</v>
       </c>
       <c r="T41" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
@@ -2379,7 +2379,7 @@
         <v>1</v>
       </c>
       <c r="I42" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" s="2" t="n">
         <v>0</v>
@@ -2397,13 +2397,13 @@
         <v>0</v>
       </c>
       <c r="O42" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P42" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q42" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R42" s="2" t="n">
         <v>0</v>
@@ -2428,55 +2428,55 @@
         <v>0</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E43" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H43" s="2" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I43" s="2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J43" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K43" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L43" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M43" s="2" t="n">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="N43" s="2" t="n">
         <v>2</v>
       </c>
       <c r="O43" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P43" s="2" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q43" s="2" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="R43" s="2" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="S43" s="2" t="n">
         <v>0</v>
       </c>
       <c r="T43" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">
@@ -2492,49 +2492,49 @@
         <v>0</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F44" s="2" t="n">
         <v>4</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H44" s="2" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I44" s="2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J44" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K44" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L44" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M44" s="2" t="n">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="N44" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O44" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P44" s="2" t="n">
         <v>24</v>
       </c>
       <c r="Q44" s="2" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="R44" s="2" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="S44" s="2" t="n">
         <v>1</v>
@@ -2571,10 +2571,10 @@
         <v>2</v>
       </c>
       <c r="I45" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K45" s="2" t="n">
         <v>0</v>
@@ -2583,10 +2583,10 @@
         <v>0</v>
       </c>
       <c r="M45" s="2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N45" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O45" s="2" t="n">
         <v>0</v>
@@ -2595,7 +2595,7 @@
         <v>2</v>
       </c>
       <c r="Q45" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R45" s="2" t="n">
         <v>1</v>
@@ -2620,25 +2620,25 @@
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G46" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H46" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I46" t="n">
         <v>2</v>
       </c>
       <c r="J46" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K46" t="n">
         <v>0</v>
@@ -2647,19 +2647,19 @@
         <v>0</v>
       </c>
       <c r="M46" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N46" t="n">
         <v>0</v>
       </c>
       <c r="O46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P46" t="n">
         <v>6</v>
       </c>
       <c r="Q46" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R46" t="n">
         <v>0</v>

</xml_diff>